<commit_message>
before exploring the probibality function os a Dl model for LIME
</commit_message>
<xml_diff>
--- a/heartDisease/Feature Exploration.xlsx
+++ b/heartDisease/Feature Exploration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Comsats\python\heartDiseasePrediction\heartDisease\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59011706-064F-4339-BE0F-847F2C5B21BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21ACF6E-7D9B-42CF-BC5D-13BBFF1000E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Features Level 0" sheetId="3" r:id="rId1"/>
@@ -994,22 +994,22 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1018,26 +1018,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1060,10 +1045,25 @@
     <xf numFmtId="10" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1379,7 +1379,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1:G1"/>
+      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1407,37 +1407,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:55" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="13"/>
+      <c r="C1" s="20"/>
       <c r="D1" s="9"/>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
       <c r="H1" s="9"/>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
       <c r="L1" s="9"/>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
       <c r="P1" s="9"/>
-      <c r="Q1" s="11" t="s">
+      <c r="Q1" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
@@ -1476,7 +1476,7 @@
       <c r="BC1" s="2"/>
     </row>
     <row r="2" spans="1:55" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
+      <c r="A2" s="21"/>
       <c r="B2" s="4" t="s">
         <v>93</v>
       </c>
@@ -2544,16 +2544,16 @@
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -3305,649 +3305,655 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F38"/>
+      <selection activeCell="B3" sqref="B3:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="60" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="60" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="12" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="C2" s="19">
+      <c r="C2" s="14">
         <v>2021</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="23">
         <v>2023</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="15" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="20" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="15" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="20" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="15" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25"/>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
       <c r="E6" s="25"/>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="14" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="23">
         <v>2022</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="20" t="s">
+      <c r="E7" s="23"/>
+      <c r="F7" s="15" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="20" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="15" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="20" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="15" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25"/>
       <c r="B10" s="25"/>
       <c r="C10" s="25"/>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="14" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="14">
         <v>2022</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19" t="s">
+      <c r="D11" s="14"/>
+      <c r="E11" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="F11" s="19"/>
-    </row>
-    <row r="12" spans="1:6" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="14">
         <v>2019</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19" t="s">
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="F12" s="19"/>
-    </row>
-    <row r="13" spans="1:6" ht="255.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="14">
         <v>2022</v>
       </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19" t="s">
+      <c r="D13" s="14"/>
+      <c r="E13" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="F13" s="19"/>
-    </row>
-    <row r="14" spans="1:6" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="14">
         <v>2020</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19" t="s">
+      <c r="D14" s="14"/>
+      <c r="E14" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="F14" s="19"/>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="F14" s="14"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="23">
         <v>2020</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="20" t="s">
+      <c r="E15" s="23"/>
+      <c r="F15" s="15" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="20" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="15" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="20" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="15" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="20" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="15" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="20" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="15" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25"/>
       <c r="B20" s="25"/>
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="14" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="18" t="s">
+    <row r="21" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="14">
         <v>2022</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="16">
         <v>0.89</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
         <v>191</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="C22" s="24">
+      <c r="C22" s="23">
         <v>2020</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="D22" s="23" t="s">
         <v>193</v>
       </c>
-      <c r="E22" s="24" t="s">
+      <c r="E22" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="F22" s="15" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="25"/>
       <c r="B23" s="25"/>
       <c r="C23" s="25"/>
       <c r="D23" s="25"/>
       <c r="E23" s="25"/>
-      <c r="F23" s="19" t="s">
+      <c r="F23" s="14" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="18" t="s">
+    <row r="24" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="14">
         <v>2020</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="F24" s="22">
+      <c r="F24" s="17">
         <v>0.98199999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="18" t="s">
+    <row r="25" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="C25" s="19">
+      <c r="C25" s="14">
         <v>2019</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="F25" s="22">
+      <c r="F25" s="17">
         <v>0.98</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="18" t="s">
+    <row r="26" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="C26" s="19">
+      <c r="C26" s="14">
         <v>2023</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="F26" s="22">
+      <c r="F26" s="17">
         <v>0.99580000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="18" t="s">
+    <row r="27" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="C27" s="19">
+      <c r="C27" s="14">
         <v>2023</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="F27" s="22">
+      <c r="F27" s="17">
         <v>0.93</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="18" t="s">
+    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="14" t="s">
         <v>213</v>
       </c>
-      <c r="C28" s="19">
+      <c r="C28" s="14">
         <v>2023</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D28" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="E28" s="19" t="s">
+      <c r="E28" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="F28" s="22">
+      <c r="F28" s="17">
         <v>0.98599999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="240.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="18" t="s">
+    <row r="29" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="14" t="s">
         <v>216</v>
       </c>
-      <c r="C29" s="19">
+      <c r="C29" s="14">
         <v>2021</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="E29" s="19" t="s">
+      <c r="E29" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="F29" s="21">
+      <c r="F29" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="18" t="s">
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="C30" s="19">
+      <c r="C30" s="14">
         <v>2021</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D30" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="E30" s="19" t="s">
+      <c r="E30" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="F30" s="21">
+      <c r="F30" s="16">
         <v>0.75</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="18" t="s">
+    <row r="31" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="B31" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="C31" s="19">
+      <c r="C31" s="14">
         <v>2023</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="E31" s="14" t="s">
         <v>225</v>
       </c>
-      <c r="F31" s="19"/>
-    </row>
-    <row r="32" spans="1:6" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="18" t="s">
+      <c r="F31" s="14"/>
+    </row>
+    <row r="32" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="B32" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="C32" s="19">
+      <c r="C32" s="14">
         <v>2020</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="E32" s="19" t="s">
+      <c r="E32" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="F32" s="22">
+      <c r="F32" s="17">
         <v>0.98499999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="18" t="s">
+    <row r="33" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="C33" s="19">
+      <c r="C33" s="14">
         <v>2020</v>
       </c>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="14" t="s">
         <v>232</v>
       </c>
-      <c r="E33" s="19" t="s">
+      <c r="E33" s="14" t="s">
         <v>233</v>
       </c>
-      <c r="F33" s="22">
+      <c r="F33" s="17">
         <v>0.86599999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="18" t="s">
+    <row r="34" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="14" t="s">
         <v>235</v>
       </c>
-      <c r="C34" s="19">
+      <c r="C34" s="14">
         <v>2019</v>
       </c>
-      <c r="D34" s="19" t="s">
+      <c r="D34" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="E34" s="19" t="s">
+      <c r="E34" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="F34" s="22">
+      <c r="F34" s="17">
         <v>0.88700000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="18" t="s">
+    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="C35" s="19">
+      <c r="C35" s="14">
         <v>2016</v>
       </c>
-      <c r="D35" s="19" t="s">
+      <c r="D35" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="E35" s="19" t="s">
+      <c r="E35" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="F35" s="22">
+      <c r="F35" s="17">
         <v>0.86699999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="18" t="s">
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="C36" s="19">
+      <c r="C36" s="14">
         <v>2015</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="E36" s="19" t="s">
+      <c r="E36" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="F36" s="19"/>
-    </row>
-    <row r="37" spans="1:6" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="18" t="s">
+      <c r="F36" s="14"/>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="13" t="s">
         <v>244</v>
       </c>
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="C37" s="19">
+      <c r="C37" s="14">
         <v>2023</v>
       </c>
-      <c r="D37" s="19" t="s">
+      <c r="D37" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="E37" s="19" t="s">
+      <c r="E37" s="14" t="s">
         <v>246</v>
       </c>
-      <c r="F37" s="19" t="s">
+      <c r="F37" s="14" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="18" t="s">
+    <row r="38" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="C38" s="19">
+      <c r="C38" s="14">
         <v>2010</v>
       </c>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="E38" s="19" t="s">
+      <c r="E38" s="14" t="s">
         <v>250</v>
       </c>
-      <c r="F38" s="22">
+      <c r="F38" s="17">
         <v>0.52329999999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
     <mergeCell ref="A15:A20"/>
     <mergeCell ref="B15:B20"/>
     <mergeCell ref="C15:C20"/>
     <mergeCell ref="D15:D20"/>
     <mergeCell ref="E15:E20"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="E3:E6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>